<commit_message>
project plan update with status
</commit_message>
<xml_diff>
--- a/project_plan.xlsx
+++ b/project_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanjeev\VNIT_CLASSES\SEM2-WORK-GIT\Model_Mavericks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D36357D2-FDCF-4B61-ADDA-E6AB2004DF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CDB0A3-134E-4AE4-A751-EDB9907035AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17172" yWindow="936" windowWidth="19416" windowHeight="10296" activeTab="1" xr2:uid="{50C1A3E4-E93F-4077-BA02-2B13CAB7060D}"/>
+    <workbookView xWindow="5805" yWindow="1785" windowWidth="16200" windowHeight="9270" activeTab="1" xr2:uid="{50C1A3E4-E93F-4077-BA02-2B13CAB7060D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Phase 1: Planning &amp; Setup (Week 1)</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>Ruturaj</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -304,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -313,9 +319,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -756,10 +759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABCA154-9E3F-4E89-800A-1E328C148A12}">
-  <dimension ref="B2:C17"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,100 +771,109 @@
     <col min="3" max="3" width="69.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -869,7 +881,7 @@
       <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>